<commit_message>
Quick Hack to include working hour update
</commit_message>
<xml_diff>
--- a/Files/Sample Excel.xlsx
+++ b/Files/Sample Excel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arian\Documents\VersaFleet\NTT\0101 Rename\rename-drivers-vehicles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arian\Documents\VersaFleet\NTT\0101 Rename\rename-drivers-vehicles\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DC9C6F15-03B6-4EC5-8CFB-BC881C3211C6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9371833-E11C-4592-AE64-CDC0FE94FB17}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11496" windowHeight="8364" xr2:uid="{C3A278C4-6E47-48CC-A8AD-1974F626DBC5}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11490" windowHeight="8370" xr2:uid="{C3A278C4-6E47-48CC-A8AD-1974F626DBC5}"/>
   </bookViews>
   <sheets>
     <sheet name="vehicle" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>Driver ID</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t>Tan Mobile</t>
+  </si>
+  <si>
+    <t>Time Slot</t>
   </si>
 </sst>
 </file>
@@ -431,18 +434,18 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1048576"/>
+      <selection activeCell="E2" sqref="E1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -456,7 +459,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>5678</v>
       </c>
@@ -477,22 +480,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1340918F-6B66-42D6-A26A-052B9FD62911}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="G1" sqref="G1:G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -511,8 +514,11 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1234</v>
       </c>
@@ -530,6 +536,9 @@
       </c>
       <c r="F2" t="s">
         <v>7</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>